<commit_message>
Journal de travail - Update 12.03.20
</commit_message>
<xml_diff>
--- a/Informations/Journal de travail.xlsx
+++ b/Informations/Journal de travail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Qui</t>
   </si>
@@ -751,7 +751,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,17 +958,31 @@
     </row>
     <row r="8" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="B8" s="13">
+        <v>43902</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.67708333333333337</v>
+      </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>

</xml_diff>

<commit_message>
Création du Menu Principale
</commit_message>
<xml_diff>
--- a/Informations/Journal de travail.xlsx
+++ b/Informations/Journal de travail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Qui</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Création des sprints pour chaques semaines</t>
+  </si>
+  <si>
+    <t>CLion</t>
+  </si>
+  <si>
+    <t>Programmation du jeu</t>
+  </si>
+  <si>
+    <t>Création des différentes fonctions</t>
   </si>
 </sst>
 </file>
@@ -751,7 +760,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,17 +995,29 @@
     </row>
     <row r="9" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="13">
+        <v>43902</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.6777777777777777</v>
+      </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
+        <v>-0.6777777777777777</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>

</xml_diff>

<commit_message>
Création fonction des règles + Update Journal de travail 13.03.20 + Modifications mineures - Visuels
</commit_message>
<xml_diff>
--- a/Informations/Journal de travail.xlsx
+++ b/Informations/Journal de travail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Qui</t>
   </si>
@@ -760,7 +760,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,17 +1023,31 @@
     </row>
     <row r="10" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="13">
+        <v>43903</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
+        <v>0.10069444444444436</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -1164,7 +1178,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f ca="1">TODAY()</f>
-        <v>43902</v>
+        <v>43903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal de travail - Update 13.03.20 + Optimisations
</commit_message>
<xml_diff>
--- a/Informations/Journal de travail.xlsx
+++ b/Informations/Journal de travail.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel.MACHADO-PERE\Documents\GitHub\Bataille-Navale\Informations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Bataille-Navale\Informations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C576B6-AEF2-421D-8C21-DC6C4881BB02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="2415" windowWidth="21600" windowHeight="11835"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
     <t>Qui</t>
   </si>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -756,11 +757,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,31 +1052,57 @@
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="B11" s="13">
+        <v>43903</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="E11" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="13">
+        <v>43903</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0.86458333333333337</v>
+      </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
+        <v>-0.86458333333333337</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>

</xml_diff>

<commit_message>
Journal de Travail - Update 14.03.20
</commit_message>
<xml_diff>
--- a/Informations/Journal de travail.xlsx
+++ b/Informations/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Bataille-Navale\Informations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C576B6-AEF2-421D-8C21-DC6C4881BB02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84282F5F-D903-4A19-8C09-91A51F35C6C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
   <si>
     <t>Qui</t>
   </si>
@@ -761,7 +761,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I15" sqref="I15:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,10 +1086,12 @@
       <c r="C12" s="11">
         <v>0.86458333333333337</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="11">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
-        <v>-0.86458333333333337</v>
+        <v>9.375E-2</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>21</v>
@@ -1106,17 +1108,31 @@
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="B13" s="13">
+        <v>43904</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
@@ -1205,7 +1221,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f ca="1">TODAY()</f>
-        <v>43903</v>
+        <v>43904</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour des commentaires
</commit_message>
<xml_diff>
--- a/Informations/Journal de travail.xlsx
+++ b/Informations/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Bataille-Navale\Informations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5ADF7D-C9F1-4F66-B2FC-D4099601A22E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8D0F4F-CCF7-4191-AC26-E3599B910B90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>Qui</t>
   </si>
@@ -761,7 +761,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,17 +1136,31 @@
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="13">
+        <v>43907</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.61319444444444449</v>
+      </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
+        <v>2.9861111111111116E-2</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -1221,7 +1235,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f ca="1">TODAY()</f>
-        <v>43904</v>
+        <v>43907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>